<commit_message>
SEK framework new ON
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK_MainChecks.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9600" windowHeight="12015"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9600" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Currency">MainChecks!$U$4</definedName>
-    <definedName name="FirstIndex">MainChecks!$K$10</definedName>
+    <definedName name="FirstIndex">MainChecks!$K$9</definedName>
     <definedName name="FuturesDates">MainChecks!$C$15:$C$18</definedName>
     <definedName name="FuturesTable">MainChecks!$A$4:$H$13</definedName>
     <definedName name="IMMFutures">MainChecks!$D$15:$D$18</definedName>
@@ -24,7 +24,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+  <si>
+    <t>ObjectID</t>
+  </si>
   <si>
     <t>Trigger</t>
   </si>
@@ -44,12 +47,21 @@
     <t>RIC</t>
   </si>
   <si>
+    <t>Curves Checks</t>
+  </si>
+  <si>
     <t>Currency</t>
   </si>
   <si>
     <t>MarketData Checks</t>
   </si>
   <si>
+    <t>Reference Date</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
     <t>Info</t>
   </si>
   <si>
@@ -158,9 +170,6 @@
     <t>6AB</t>
   </si>
   <si>
-    <t>YBAM5</t>
-  </si>
-  <si>
     <t>Expiry-Value Date</t>
   </si>
   <si>
@@ -176,37 +185,19 @@
     <t>JGBc1</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>3S</t>
+  </si>
+  <si>
     <t>TRHK</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>3S</t>
-  </si>
-  <si>
     <t>Shibor</t>
   </si>
   <si>
     <t>SEK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           </t>
-  </si>
-  <si>
-    <t>Stibor</t>
-  </si>
-  <si>
-    <t>Curve Checks</t>
-  </si>
-  <si>
-    <t>Object ID</t>
-  </si>
-  <si>
-    <t>Reference Date</t>
-  </si>
-  <si>
-    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -224,7 +215,7 @@
     <numFmt numFmtId="171" formatCode="ddd\,\ dd\-mmm\-yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="172" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -282,8 +273,13 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,8 +321,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -381,19 +383,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -507,13 +496,42 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -532,17 +550,32 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -553,12 +586,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -568,14 +599,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -583,28 +616,22 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,77 +640,93 @@
     <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="16" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="0" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="18" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
     <cellStyle name="Migliaia_AZIONI" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="11"/>
-    <cellStyle name="Normal 3" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="9"/>
     <cellStyle name="Normale_AZIONI" xfId="3"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Note 2" xfId="9"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
     <cellStyle name="result" xfId="5"/>
     <cellStyle name="Valuta (0)_AZIONI" xfId="6"/>
@@ -772,28 +815,22 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:16:44</v>
+        <v>Updated at 10:47:18</v>
         <stp/>
-        <stp>{6EE91872-E1FD-40BA-ABD5-4968E8047AE5}</stp>
-        <tr r="P7" s="2"/>
+        <stp>{292E977D-567D-40EF-A06F-5066420396E1}</stp>
+        <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 11:16:44</v>
+        <v>Updated at 10:33:08</v>
         <stp/>
-        <stp>{32CF7FD2-B885-4A55-BD84-E97411878549}</stp>
-        <tr r="Q6" s="2"/>
+        <stp>{B91E27F1-45EF-4EE7-87AD-B570C22D5925}</stp>
+        <tr r="P6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 11:16:44</v>
+        <v>Updated at 09:15:43</v>
         <stp/>
-        <stp>{6B37FF9D-A0C6-4B80-895C-0326E41EDD99}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 11:16:44</v>
-        <stp/>
-        <stp>{C9B8A749-B5DD-471B-A7C6-A63DC7F594AB}</stp>
-        <tr r="Q5" s="2"/>
+        <stp>{5ECB78B6-4A9C-4D3F-AF93-258D3BF9A2E1}</stp>
+        <tr r="Q6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1185,7 +1222,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ101"/>
+  <dimension ref="A1:AJ103"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
@@ -1196,7 +1233,7 @@
     <col min="1" max="1" width="4" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="2" width="5" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="10" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="7" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="6" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="3" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="4" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="5" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -1209,7 +1246,8 @@
     <col min="14" max="15" width="7" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="16" max="16" width="20.28515625" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="20.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="2.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9.28515625" style="2"/>
@@ -1272,15 +1310,13 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S2" s="1"/>
-      <c r="T2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="19">
-        <v>41989.469895833332</v>
-      </c>
+      <c r="T2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="18"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -1308,17 +1344,17 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="16"/>
+      <c r="K3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
       <c r="R3" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1340,56 +1376,56 @@
       <c r="AJ3" s="3"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="46" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="18" t="s">
+      <c r="K4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>54</v>
+      <c r="U4" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1408,57 +1444,57 @@
       <c r="AJ4" s="3"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="49" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="26">
+      <c r="K5" s="24" t="str">
         <f>VLOOKUP(Currency,FuturesTable,3,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="28">
-        <v>0</v>
-      </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="29" t="str">
+        <v>FGBLc1</v>
+      </c>
+      <c r="L5" s="25">
+        <v>42069</v>
+      </c>
+      <c r="M5" s="26">
+        <v>155.06</v>
+      </c>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 11:16:44</v>
+        <v>Updated at 10:47:18</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" s="12" t="str">
+      <c r="T5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="11" t="str">
         <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
         <v>1_52 / 1.5.0 / 1.5</v>
       </c>
@@ -1479,58 +1515,67 @@
       <c r="AJ5" s="3"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="A6" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="48" t="s">
         <v>32</v>
       </c>
+      <c r="F6" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>36</v>
+      </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="47">
-        <v>42166</v>
-      </c>
-      <c r="M6" s="48">
-        <v>97.59</v>
-      </c>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="31" t="str">
-        <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 11:16:44</v>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21" t="str">
+        <f>Currency&amp;VLOOKUP(Currency,FuturesTable,5,0)&amp;VLOOKUP(Currency,FuturesTable,6,0)&amp;"10Y"</f>
+        <v>SEKAB3S10Y</v>
+      </c>
+      <c r="L6" s="22">
+        <v>41990</v>
+      </c>
+      <c r="M6" s="30" t="str">
+        <f>N6&amp;"/"&amp;O6</f>
+        <v>1.22/1.27</v>
+      </c>
+      <c r="N6" s="28">
+        <v>1.22</v>
+      </c>
+      <c r="O6" s="28">
+        <v>1.27</v>
+      </c>
+      <c r="P6" s="28" t="str">
+        <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
+        <v>Updated at 10:33:08</v>
+      </c>
+      <c r="Q6" s="29" t="str">
+        <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
+        <v>Updated at 09:15:43</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="U6" s="12">
+      <c r="T6" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>670</v>
+        <v>562</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1548,58 +1593,44 @@
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="37" t="s">
+    <row r="7" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="23" t="str">
-        <f>Currency&amp;VLOOKUP(Currency,FuturesTable,5,0)&amp;VLOOKUP(Currency,FuturesTable,6,0)&amp;"10Y"</f>
-        <v>SEKAB3S10Y</v>
-      </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="33" t="str">
-        <f>N7&amp;"/"&amp;O7</f>
-        <v>1.22/1.27</v>
-      </c>
-      <c r="N7" s="30">
-        <v>1.22</v>
-      </c>
-      <c r="O7" s="30">
-        <v>1.27</v>
-      </c>
-      <c r="P7" s="30" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 11:16:44</v>
-      </c>
-      <c r="Q7" s="31" t="str">
-        <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 11:16:44</v>
-      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="15"/>
       <c r="R7" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1620,44 +1651,50 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
     </row>
-    <row r="8" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="37" t="s">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>32</v>
+      <c r="H8" s="49" t="s">
+        <v>36</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="16"/>
+      <c r="K8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="R8" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1679,49 +1716,53 @@
       <c r="AJ8" s="3"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="37" t="s">
+      <c r="A9" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>34</v>
+      <c r="G9" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>38</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="18" t="s">
-        <v>8</v>
+      <c r="K9" s="60" t="str">
+        <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
+        <v>Sekibor3M</v>
+      </c>
+      <c r="L9" s="57">
+        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>41989</v>
+      </c>
+      <c r="M9" s="58">
+        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="59" t="str">
+        <f>IF(AND(ISERROR(L9),ISERROR(M9)),_xll.ohRangeRetrieveError(L9)&amp;" "&amp;_xll.ohRangeRetrieveError(M9),IF(ISERROR(L9),_xll.ohRangeRetrieveError(L9),_xll.ohRangeRetrieveError(M9)))</f>
+        <v/>
       </c>
       <c r="R9" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1743,53 +1784,53 @@
       <c r="AJ9" s="3"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="45" t="s">
+      <c r="A10" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="48" t="s">
         <v>53</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>56</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="22" t="str">
-        <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
-        <v>SekStibor3M</v>
-      </c>
-      <c r="L10" s="49" t="e">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+      <c r="K10" s="21" t="str">
+        <f>UPPER(Currency)&amp;"STD"</f>
+        <v>SEKSTD</v>
+      </c>
+      <c r="L10" s="22" t="e">
+        <f>_xll.qlTermStructureReferenceDate(K10,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M10" s="32" t="e">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+      <c r="M10" s="23" t="e">
+        <f>_xll.qlYieldTSDiscount(K10,L10)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="34" t="str">
-        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v>qlLastFixingQuoteReferenceDate - ObjectHandler error: attempt to retrieve object with unknown ID 'SekStibor3MLastFixing_Quote' qlQuoteValue - ObjectHandler error: attempt to retrieve object with unknown ID 'SekStibor3MLastFixing_Quote'</v>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="31" t="str">
+        <f ca="1">IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
+        <v/>
       </c>
       <c r="R10" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -1811,53 +1852,53 @@
       <c r="AJ10" s="3"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="45" t="s">
-        <v>33</v>
+      <c r="A11" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>37</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="23" t="str">
-        <f>UPPER(Currency)&amp;"STD"</f>
-        <v>SEKSTD</v>
-      </c>
-      <c r="L11" s="50" t="e">
+      <c r="K11" s="21" t="str">
+        <f>UPPER(Currency)&amp;"TN"</f>
+        <v>SEKTN</v>
+      </c>
+      <c r="L11" s="22">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M11" s="25" t="e">
+        <v>41992</v>
+      </c>
+      <c r="M11" s="23">
         <f>_xll.qlYieldTSDiscount(K11,L11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="35" t="str">
-        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v>1</v>
+      </c>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="31" t="str">
+        <f>IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+        <v/>
       </c>
       <c r="R11" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -1880,50 +1921,52 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="45" t="s">
-        <v>56</v>
+      <c r="G12" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="23" t="str">
-        <f>UPPER(Currency)&amp;"ON"</f>
-        <v>SEKON</v>
-      </c>
-      <c r="L12" s="50" t="e">
+      <c r="K12" s="21" t="str">
+        <f>UPPER(Currency)&amp;"1M"</f>
+        <v>SEK1M</v>
+      </c>
+      <c r="L12" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M12" s="25" t="e">
+      <c r="M12" s="23" t="e">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="36" t="str">
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="31" t="str">
         <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R12" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -1945,47 +1988,47 @@
       <c r="AJ12" s="3"/>
     </row>
     <row r="13" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="10" t="s">
+      <c r="A13" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11" t="s">
-        <v>32</v>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54" t="s">
+        <v>36</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="23" t="str">
-        <f>UPPER(Currency)&amp;"1M"</f>
-        <v>SEK1M</v>
-      </c>
-      <c r="L13" s="50" t="e">
+      <c r="K13" s="21" t="str">
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>SEK3M</v>
+      </c>
+      <c r="L13" s="22" t="e">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M13" s="25" t="e">
+      <c r="M13" s="23" t="e">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="36" t="str">
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="32" t="str">
         <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R13" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -2017,27 +2060,27 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="23" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>SEK3M</v>
-      </c>
-      <c r="L14" s="50" t="e">
+      <c r="K14" s="39" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>SEK6M</v>
+      </c>
+      <c r="L14" s="40" t="e">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M14" s="25" t="e">
+      <c r="M14" s="41" t="e">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="36" t="str">
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="42" t="str">
         <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v/>
       </c>
       <c r="R14" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -2058,12 +2101,12 @@
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="33">
         <f t="array" ref="C15:C18">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B15:B18)</f>
         <v>41990</v>
       </c>
@@ -2076,28 +2119,16 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="23" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>SEK6M</v>
-      </c>
-      <c r="L15" s="50" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M15" s="25" t="e">
-        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="36" t="str">
-        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>9</v>
+      <c r="J15" s="9"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -2118,12 +2149,12 @@
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
     </row>
-    <row r="16" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="41" t="b">
+      <c r="B16" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="34">
         <v>42081</v>
       </c>
       <c r="D16" s="8" t="str">
@@ -2134,17 +2165,15 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="44"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -2166,10 +2195,10 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
-      <c r="B17" s="41" t="b">
+      <c r="B17" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="34">
         <v>42172</v>
       </c>
       <c r="D17" s="8" t="str">
@@ -2210,13 +2239,13 @@
     </row>
     <row r="18" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="42" t="b">
+      <c r="B18" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="35">
         <v>42263</v>
       </c>
-      <c r="D18" s="11" t="str">
+      <c r="D18" s="10" t="str">
         <v>-U5</v>
       </c>
       <c r="E18" s="3"/>
@@ -3068,7 +3097,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
+      <c r="R40" s="3"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
@@ -3098,14 +3127,14 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
@@ -5226,15 +5255,15 @@
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="3"/>
-      <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-      <c r="Q97" s="3"/>
-      <c r="R97" s="3"/>
+      <c r="J97" s="55"/>
+      <c r="K97" s="55"/>
+      <c r="L97" s="55"/>
+      <c r="M97" s="55"/>
+      <c r="N97" s="55"/>
+      <c r="O97" s="55"/>
+      <c r="P97" s="55"/>
+      <c r="Q97" s="55"/>
+      <c r="R97" s="55"/>
       <c r="S97" s="3"/>
       <c r="T97" s="3"/>
       <c r="U97" s="3"/>
@@ -5264,15 +5293,15 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-      <c r="Q98" s="3"/>
-      <c r="R98" s="3"/>
+      <c r="J98" s="55"/>
+      <c r="K98" s="55"/>
+      <c r="L98" s="55"/>
+      <c r="M98" s="55"/>
+      <c r="N98" s="55"/>
+      <c r="O98" s="55"/>
+      <c r="P98" s="55"/>
+      <c r="Q98" s="55"/>
+      <c r="R98" s="55"/>
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -5302,15 +5331,15 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
+      <c r="J99" s="43"/>
+      <c r="K99" s="43"/>
+      <c r="L99" s="43"/>
+      <c r="M99" s="43"/>
+      <c r="N99" s="43"/>
+      <c r="O99" s="43"/>
+      <c r="P99" s="43"/>
+      <c r="Q99" s="43"/>
+      <c r="R99" s="43"/>
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -5340,15 +5369,6 @@
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="3"/>
-      <c r="L100" s="3"/>
-      <c r="M100" s="3"/>
-      <c r="N100" s="3"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-      <c r="Q100" s="3"/>
-      <c r="R100" s="3"/>
       <c r="S100" s="3"/>
       <c r="T100" s="3"/>
       <c r="U100" s="3"/>
@@ -5368,7 +5388,7 @@
       <c r="AI100" s="3"/>
       <c r="AJ100" s="3"/>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5377,22 +5397,42 @@
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+      <c r="O101" s="2"/>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
+      <c r="R101" s="2"/>
+      <c r="S101" s="55"/>
+    </row>
+    <row r="102" spans="1:36" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2"/>
+      <c r="S102" s="55"/>
+    </row>
+    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A103" s="43"/>
+      <c r="B103" s="43"/>
+      <c r="C103" s="43"/>
+      <c r="D103" s="43"/>
+      <c r="E103" s="43"/>
+      <c r="F103" s="43"/>
+      <c r="G103" s="43"/>
+      <c r="H103" s="43"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6">
-      <formula1>IMMFutures</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4">
       <formula1>"EUR,USD,GBP,JPY,CHF,AUD,CNY,CNH,HKD,RMB,SEK"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
SEK framework - 6MCurve
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK_MainChecks.xlsx
@@ -815,22 +815,22 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:47:18</v>
+        <v>Updated at 11:45:49</v>
         <stp/>
-        <stp>{292E977D-567D-40EF-A06F-5066420396E1}</stp>
-        <tr r="Q5" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 10:33:08</v>
-        <stp/>
-        <stp>{B91E27F1-45EF-4EE7-87AD-B570C22D5925}</stp>
+        <stp>{91777A41-E1F4-4590-A1F0-2644D245C61B}</stp>
         <tr r="P6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:15:43</v>
+        <v>Updated at 09:52:05</v>
         <stp/>
-        <stp>{5ECB78B6-4A9C-4D3F-AF93-258D3BF9A2E1}</stp>
+        <stp>{325EA38B-8E9F-4B2D-96D3-051E34C0327D}</stp>
         <tr r="Q6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:34:26</v>
+        <stp/>
+        <stp>{9DDD02AE-8C60-4549-A705-CFB6489716F0}</stp>
+        <tr r="Q5" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1478,14 +1478,14 @@
         <v>42069</v>
       </c>
       <c r="M5" s="26">
-        <v>155.06</v>
+        <v>155.18</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 10:47:18</v>
+        <v>Updated at 12:34:26</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1546,25 +1546,25 @@
         <v>SEKAB3S10Y</v>
       </c>
       <c r="L6" s="22">
-        <v>41990</v>
+        <v>41991</v>
       </c>
       <c r="M6" s="30" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>1.22/1.27</v>
+        <v>1.2225/1.2725</v>
       </c>
       <c r="N6" s="28">
-        <v>1.22</v>
+        <v>1.2224999999999999</v>
       </c>
       <c r="O6" s="28">
-        <v>1.27</v>
+        <v>1.2725</v>
       </c>
       <c r="P6" s="28" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Updated at 10:33:08</v>
+        <v>Updated at 11:45:49</v>
       </c>
       <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Updated at 09:15:43</v>
+        <v>Updated at 09:52:05</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>562</v>
+        <v>702</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1748,11 +1748,11 @@
       </c>
       <c r="L9" s="57">
         <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>41989</v>
+        <v>41991</v>
       </c>
       <c r="M9" s="58">
         <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>2.5999999999999999E-3</v>
+        <v>2.5800000000000003E-3</v>
       </c>
       <c r="N9" s="58"/>
       <c r="O9" s="58"/>
@@ -1827,7 +1827,7 @@
       <c r="P10" s="23"/>
       <c r="Q10" s="31" t="str">
         <f ca="1">IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
-        <v/>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1879,12 +1879,12 @@
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
       <c r="K11" s="21" t="str">
-        <f>UPPER(Currency)&amp;"TN"</f>
-        <v>SEKTN</v>
+        <f>UPPER(Currency)&amp;"ON"</f>
+        <v>SEKON</v>
       </c>
       <c r="L11" s="22">
         <f>_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
-        <v>41992</v>
+        <v>41995</v>
       </c>
       <c r="M11" s="23">
         <f>_xll.qlYieldTSDiscount(K11,L11)</f>
@@ -1963,7 +1963,7 @@
       <c r="P12" s="23"/>
       <c r="Q12" s="31" t="str">
         <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v/>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R12" s="8" t="s">
         <v>13</v>
@@ -2025,7 +2025,7 @@
       <c r="P13" s="23"/>
       <c r="Q13" s="32" t="str">
         <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v/>
+        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -2064,9 +2064,9 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>SEK6M</v>
       </c>
-      <c r="L14" s="40" t="e">
+      <c r="L14" s="40">
         <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41995</v>
       </c>
       <c r="M14" s="41" t="e">
         <f>_xll.qlYieldTSDiscount(K14,L14)</f>
@@ -2077,7 +2077,7 @@
       <c r="P14" s="41"/>
       <c r="Q14" s="42" t="str">
         <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v/>
+        <v>qlYieldTSDiscount - 1st instrument (maturity: December 23rd, 2014) has an invalid quote</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>13</v>
@@ -2108,11 +2108,11 @@
       </c>
       <c r="C15" s="33">
         <f t="array" ref="C15:C18">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B15:B18)</f>
-        <v>41990</v>
+        <v>42081</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="array" ref="D15:D18">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>-Z4</v>
+        <v>-H5</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2155,10 +2155,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="34">
-        <v>42081</v>
+        <v>42172</v>
       </c>
       <c r="D16" s="8" t="str">
-        <v>-H5</v>
+        <v>-M5</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2199,10 +2199,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="34">
-        <v>42172</v>
+        <v>42263</v>
       </c>
       <c r="D17" s="8" t="str">
-        <v>-M5</v>
+        <v>-U5</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2243,10 +2243,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="35">
-        <v>42263</v>
+        <v>42354</v>
       </c>
       <c r="D18" s="10" t="str">
-        <v>-U5</v>
+        <v>-Z5</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -5445,7 +5445,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5465,12 +5465,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5490,7 +5490,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
SEK Framework - STD Curve
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/SEK_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/SEK_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9600" windowHeight="12600"/>
+    <workbookView visibility="hidden" xWindow="-15" yWindow="45" windowWidth="9600" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
   <si>
     <t>ObjectID</t>
   </si>
@@ -815,21 +815,21 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:45:49</v>
+        <v>Updated at 15:35:39</v>
         <stp/>
-        <stp>{91777A41-E1F4-4590-A1F0-2644D245C61B}</stp>
+        <stp>{4F5FD10D-8768-4E20-8610-4638D04F9844}</stp>
         <tr r="P6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:52:05</v>
+        <v>Updated at 14:37:52</v>
         <stp/>
-        <stp>{325EA38B-8E9F-4B2D-96D3-051E34C0327D}</stp>
+        <stp>{AE8188EC-8156-47F1-80BB-FCD5546845E4}</stp>
         <tr r="Q6" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:34:26</v>
+        <v>Updated at 15:38:11</v>
         <stp/>
-        <stp>{9DDD02AE-8C60-4549-A705-CFB6489716F0}</stp>
+        <stp>{E3E18B92-86D6-4C93-808F-B168A6A8FE7F}</stp>
         <tr r="Q5" s="2"/>
       </tp>
     </main>
@@ -1478,14 +1478,14 @@
         <v>42069</v>
       </c>
       <c r="M5" s="26">
-        <v>155.18</v>
+        <v>154.69</v>
       </c>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="27" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 12:34:26</v>
+        <v>Updated at 15:38:11</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1550,21 +1550,21 @@
       </c>
       <c r="M6" s="30" t="str">
         <f>N6&amp;"/"&amp;O6</f>
-        <v>1.2225/1.2725</v>
+        <v>1.2725/1.3225</v>
       </c>
       <c r="N6" s="28">
-        <v>1.2224999999999999</v>
+        <v>1.2725</v>
       </c>
       <c r="O6" s="28">
-        <v>1.2725</v>
+        <v>1.3225</v>
       </c>
       <c r="P6" s="28" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N6)</f>
-        <v>Updated at 11:45:49</v>
+        <v>Updated at 15:35:39</v>
       </c>
       <c r="Q6" s="29" t="str">
         <f>_xll.RData(K6&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L6)</f>
-        <v>Updated at 09:52:05</v>
+        <v>Updated at 14:37:52</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="U6" s="11">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>702</v>
+        <v>758</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1814,20 +1814,20 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>SEKSTD</v>
       </c>
-      <c r="L10" s="22" t="e">
+      <c r="L10" s="22">
         <f>_xll.qlTermStructureReferenceDate(K10,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M10" s="23" t="e">
+        <v>41995</v>
+      </c>
+      <c r="M10" s="23">
         <f>_xll.qlYieldTSDiscount(K10,L10)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
       <c r="Q10" s="31" t="str">
-        <f ca="1">IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <f>IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10))</f>
+        <v/>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1947,12 +1947,12 @@
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
       <c r="K12" s="21" t="str">
-        <f>UPPER(Currency)&amp;"1M"</f>
-        <v>SEK1M</v>
-      </c>
-      <c r="L12" s="22" t="e">
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>SEK3M</v>
+      </c>
+      <c r="L12" s="22">
         <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
+        <v>41995</v>
       </c>
       <c r="M12" s="23" t="e">
         <f>_xll.qlYieldTSDiscount(K12,L12)</f>
@@ -1961,9 +1961,9 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
-      <c r="Q12" s="31" t="str">
+      <c r="Q12" s="32" t="str">
         <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v>qlYieldTSDiscount - 1st instrument (maturity: January 22nd, 2015) has an invalid quote</v>
       </c>
       <c r="R12" s="8" t="s">
         <v>13</v>
@@ -2008,24 +2008,24 @@
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="21" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>SEK3M</v>
-      </c>
-      <c r="L13" s="22" t="e">
+      <c r="K13" s="39" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>SEK6M</v>
+      </c>
+      <c r="L13" s="40">
         <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M13" s="23" t="e">
+        <v>41995</v>
+      </c>
+      <c r="M13" s="41" t="e">
         <f>_xll.qlYieldTSDiscount(K13,L13)</f>
         <v>#NUM!</v>
       </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="32" t="str">
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="42" t="str">
         <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
-        <v>qlTermStructureReferenceDate - empty Handle cannot be dereferenced</v>
+        <v>qlYieldTSDiscount - 1st instrument (maturity: December 23rd, 2014) has an invalid quote</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>13</v>
@@ -2059,27 +2059,15 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="39" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>SEK6M</v>
-      </c>
-      <c r="L14" s="40">
-        <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>41995</v>
-      </c>
-      <c r="M14" s="41" t="e">
-        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="42" t="str">
-        <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
-        <v>qlYieldTSDiscount - 1st instrument (maturity: December 23rd, 2014) has an invalid quote</v>
-      </c>
-      <c r="R14" s="8" t="s">
+      <c r="J14" s="9"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="S14" s="1"/>
@@ -2101,7 +2089,7 @@
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
     </row>
-    <row r="15" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="b">
         <v>1</v>
@@ -2119,17 +2107,15 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -3059,7 +3045,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
+      <c r="R39" s="3"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
@@ -3089,14 +3075,14 @@
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
@@ -5217,15 +5203,15 @@
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
-      <c r="R96" s="3"/>
+      <c r="J96" s="55"/>
+      <c r="K96" s="55"/>
+      <c r="L96" s="55"/>
+      <c r="M96" s="55"/>
+      <c r="N96" s="55"/>
+      <c r="O96" s="55"/>
+      <c r="P96" s="55"/>
+      <c r="Q96" s="55"/>
+      <c r="R96" s="55"/>
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
       <c r="U96" s="3"/>
@@ -5293,15 +5279,15 @@
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="55"/>
-      <c r="K98" s="55"/>
-      <c r="L98" s="55"/>
-      <c r="M98" s="55"/>
-      <c r="N98" s="55"/>
-      <c r="O98" s="55"/>
-      <c r="P98" s="55"/>
-      <c r="Q98" s="55"/>
-      <c r="R98" s="55"/>
+      <c r="J98" s="43"/>
+      <c r="K98" s="43"/>
+      <c r="L98" s="43"/>
+      <c r="M98" s="43"/>
+      <c r="N98" s="43"/>
+      <c r="O98" s="43"/>
+      <c r="P98" s="43"/>
+      <c r="Q98" s="43"/>
+      <c r="R98" s="43"/>
       <c r="S98" s="3"/>
       <c r="T98" s="3"/>
       <c r="U98" s="3"/>
@@ -5331,15 +5317,6 @@
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
-      <c r="J99" s="43"/>
-      <c r="K99" s="43"/>
-      <c r="L99" s="43"/>
-      <c r="M99" s="43"/>
-      <c r="N99" s="43"/>
-      <c r="O99" s="43"/>
-      <c r="P99" s="43"/>
-      <c r="Q99" s="43"/>
-      <c r="R99" s="43"/>
       <c r="S99" s="3"/>
       <c r="T99" s="3"/>
       <c r="U99" s="3"/>
@@ -5445,7 +5422,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5465,12 +5442,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5490,7 +5467,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>